<commit_message>
Resolves #22 - added option to use custom controls location that are not columns. This function is currently not available for plate maps.
</commit_message>
<xml_diff>
--- a/Validation/test.xlsx
+++ b/Validation/test.xlsx
@@ -23,52 +23,52 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
-    <t xml:space="preserve">sample.one</t>
+    <t xml:space="preserve">sample one</t>
   </si>
   <si>
-    <t xml:space="preserve">sample.one.1</t>
+    <t xml:space="preserve">sample one.1</t>
   </si>
   <si>
-    <t xml:space="preserve">sample.two</t>
+    <t xml:space="preserve">sample two</t>
   </si>
   <si>
-    <t xml:space="preserve">NA.</t>
+    <t xml:space="preserve">NA</t>
   </si>
   <si>
-    <t xml:space="preserve">sample.three</t>
+    <t xml:space="preserve">sample three</t>
   </si>
   <si>
-    <t xml:space="preserve">sample.three.1</t>
+    <t xml:space="preserve">sample three.1</t>
   </si>
   <si>
-    <t xml:space="preserve">X9</t>
+    <t xml:space="preserve">9</t>
   </si>
   <si>
-    <t xml:space="preserve">X10</t>
+    <t xml:space="preserve">10</t>
   </si>
   <si>
-    <t xml:space="preserve">X11</t>
+    <t xml:space="preserve">11</t>
   </si>
   <si>
-    <t xml:space="preserve">X12</t>
+    <t xml:space="preserve">12</t>
   </si>
   <si>
-    <t xml:space="preserve">X3</t>
+    <t xml:space="preserve">3</t>
   </si>
   <si>
-    <t xml:space="preserve">X4</t>
+    <t xml:space="preserve">4</t>
   </si>
   <si>
-    <t xml:space="preserve">X5</t>
+    <t xml:space="preserve">5</t>
   </si>
   <si>
-    <t xml:space="preserve">X6</t>
+    <t xml:space="preserve">6</t>
   </si>
   <si>
-    <t xml:space="preserve">X7</t>
+    <t xml:space="preserve">7</t>
   </si>
   <si>
-    <t xml:space="preserve">X8</t>
+    <t xml:space="preserve">8</t>
   </si>
 </sst>
 </file>

</xml_diff>